<commit_message>
Cambio en las fechas de actividades y agrego la primera parte de los casos de uso al informe
</commit_message>
<xml_diff>
--- a/Planeacion actividades.xlsx
+++ b/Planeacion actividades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrés\Universidad\SÉPTIMO SEMESTRE\FIS\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89376C8B-40D8-4189-800B-594E1A5F9FE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C7CA7-C6E9-46A0-BFAA-6665A445022C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{37E2385D-BCEF-49EC-9252-992955D84BB6}"/>
   </bookViews>
@@ -129,6 +129,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -138,13 +145,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFE3F39-B2D0-4C8D-A05F-5AE45C56E644}">
   <dimension ref="A2:N147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,31 +474,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="3">
         <f>(SUM(E4:E7))</f>
         <v>10</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -508,95 +508,95 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="8">
+      <c r="B4" s="6"/>
+      <c r="C4" s="5">
         <v>43566</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="4">
         <v>43568</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4">
         <v>43569</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <v>43572</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="7">
+      <c r="B6" s="6"/>
+      <c r="C6" s="4">
         <v>43573</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <v>43573</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7">
+      <c r="B7" s="2"/>
+      <c r="C7" s="4">
         <v>43574</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <v>43575</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="6" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="6">
-        <f t="shared" ref="G3:G38" si="0">(SUM(E10:E13))</f>
+      <c r="G8" s="3">
+        <f t="shared" ref="G8:G38" si="0">(SUM(E10:E13))</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
@@ -607,95 +607,95 @@
         <v>7</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="8">
+      <c r="B10" s="6"/>
+      <c r="C10" s="5">
         <v>43576</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>43577</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="7">
+      <c r="B11" s="2"/>
+      <c r="C11" s="4">
         <v>43578</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="4">
         <v>43579</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="6"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="7">
+      <c r="B12" s="6"/>
+      <c r="C12" s="4">
         <v>43580</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="4">
         <v>43580</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="7">
+      <c r="B13" s="2"/>
+      <c r="C13" s="4">
         <v>43581</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="5">
         <v>43581</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -706,95 +706,95 @@
         <v>7</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="8">
+      <c r="B16" s="6"/>
+      <c r="C16" s="5">
         <v>43582</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>43585</v>
       </c>
       <c r="E16" s="1">
         <v>4</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="7">
+      <c r="B17" s="2"/>
+      <c r="C17" s="4">
         <v>43586</v>
       </c>
-      <c r="D17" s="7">
-        <v>43589</v>
+      <c r="D17" s="4">
+        <v>43592</v>
       </c>
       <c r="E17" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="6"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="7">
-        <v>43590</v>
-      </c>
-      <c r="D18" s="7">
-        <v>43591</v>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4">
+        <v>43593</v>
+      </c>
+      <c r="D18" s="4">
+        <v>43593</v>
       </c>
       <c r="E18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="6"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="7">
-        <v>43592</v>
-      </c>
-      <c r="D19" s="8">
-        <v>43592</v>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4">
+        <v>43594</v>
+      </c>
+      <c r="D19" s="5">
+        <v>43594</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="6"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="6" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
@@ -805,95 +805,95 @@
         <v>7</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="6"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="8">
-        <v>43563</v>
-      </c>
-      <c r="D22" s="7">
-        <v>43597</v>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5">
+        <v>43565</v>
+      </c>
+      <c r="D22" s="4">
+        <v>43599</v>
       </c>
       <c r="E22" s="1">
         <v>5</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="6"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="7">
-        <v>43598</v>
-      </c>
-      <c r="D23" s="7">
-        <v>43602</v>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4">
+        <v>43600</v>
+      </c>
+      <c r="D23" s="4">
+        <v>43604</v>
       </c>
       <c r="E23" s="1">
         <v>5</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="6"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="7">
-        <v>43603</v>
-      </c>
-      <c r="D24" s="7">
-        <v>43604</v>
+      <c r="B24" s="6"/>
+      <c r="C24" s="4">
+        <v>43605</v>
+      </c>
+      <c r="D24" s="4">
+        <v>43606</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="6"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="7">
-        <v>43605</v>
-      </c>
-      <c r="D25" s="8">
-        <v>43605</v>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4">
+        <v>43607</v>
+      </c>
+      <c r="D25" s="5">
+        <v>43607</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="6"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="6" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
@@ -904,95 +904,95 @@
         <v>7</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="6"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="8">
-        <v>43606</v>
-      </c>
-      <c r="D28" s="7">
-        <v>43607</v>
+      <c r="B28" s="6"/>
+      <c r="C28" s="5">
+        <v>43608</v>
+      </c>
+      <c r="D28" s="4">
+        <v>43609</v>
       </c>
       <c r="E28" s="1">
         <v>2</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="6"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="7">
-        <v>43608</v>
-      </c>
-      <c r="D29" s="7">
-        <v>43609</v>
+      <c r="B29" s="2"/>
+      <c r="C29" s="4">
+        <v>43610</v>
+      </c>
+      <c r="D29" s="4">
+        <v>43611</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="7">
-        <v>43610</v>
-      </c>
-      <c r="D30" s="7">
-        <v>43610</v>
+      <c r="B30" s="6"/>
+      <c r="C30" s="4">
+        <v>43612</v>
+      </c>
+      <c r="D30" s="4">
+        <v>43612</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="6"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="7">
-        <v>43611</v>
-      </c>
-      <c r="D31" s="8">
-        <v>43611</v>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4">
+        <v>43613</v>
+      </c>
+      <c r="D31" s="5">
+        <v>43613</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="6"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="6" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1003,95 +1003,95 @@
         <v>7</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="6"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="8">
-        <v>43612</v>
-      </c>
-      <c r="D34" s="7">
-        <v>43616</v>
+      <c r="B34" s="6"/>
+      <c r="C34" s="5">
+        <v>43614</v>
+      </c>
+      <c r="D34" s="4">
+        <v>43587</v>
       </c>
       <c r="E34" s="1">
         <v>5</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="6"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="7">
-        <v>43617</v>
-      </c>
-      <c r="D35" s="7">
-        <v>43621</v>
+      <c r="B35" s="2"/>
+      <c r="C35" s="4">
+        <v>43619</v>
+      </c>
+      <c r="D35" s="4">
+        <v>43623</v>
       </c>
       <c r="E35" s="1">
         <v>5</v>
       </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="6"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="7">
-        <v>43622</v>
-      </c>
-      <c r="D36" s="7">
-        <v>43623</v>
+      <c r="B36" s="6"/>
+      <c r="C36" s="4">
+        <v>43624</v>
+      </c>
+      <c r="D36" s="4">
+        <v>43625</v>
       </c>
       <c r="E36" s="1">
         <v>2</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="6"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="7">
-        <v>43624</v>
-      </c>
-      <c r="D37" s="8">
-        <v>43625</v>
+      <c r="B37" s="2"/>
+      <c r="C37" s="4">
+        <v>43626</v>
+      </c>
+      <c r="D37" s="5">
+        <v>43627</v>
       </c>
       <c r="E37" s="1">
         <v>2</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="6"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="6" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="1" t="s">
         <v>5</v>
       </c>
@@ -1104,15 +1104,15 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="8">
-        <v>43626</v>
-      </c>
-      <c r="D40" s="7">
-        <v>43630</v>
+      <c r="B40" s="6"/>
+      <c r="C40" s="5">
+        <v>43628</v>
+      </c>
+      <c r="D40" s="4">
+        <v>43632</v>
       </c>
       <c r="E40" s="1">
         <v>5</v>
@@ -1120,15 +1120,15 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="7">
-        <v>43631</v>
-      </c>
-      <c r="D41" s="7">
-        <v>43635</v>
+      <c r="B41" s="2"/>
+      <c r="C41" s="4">
+        <v>43633</v>
+      </c>
+      <c r="D41" s="4">
+        <v>43637</v>
       </c>
       <c r="E41" s="1">
         <v>5</v>
@@ -1136,15 +1136,15 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="7">
-        <v>43636</v>
-      </c>
-      <c r="D42" s="7">
-        <v>43636</v>
+      <c r="B42" s="6"/>
+      <c r="C42" s="4">
+        <v>43638</v>
+      </c>
+      <c r="D42" s="4">
+        <v>43638</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -1152,15 +1152,15 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="7">
-        <v>43637</v>
-      </c>
-      <c r="D43" s="8">
-        <v>43637</v>
+      <c r="B43" s="2"/>
+      <c r="C43" s="4">
+        <v>43639</v>
+      </c>
+      <c r="D43" s="5">
+        <v>43639</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="G45">
         <f>SUM(G2:G44)</f>
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1799,11 +1799,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A27:B27"/>
@@ -1811,22 +1822,11 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
INFORME: Parte faltante de open source e inicio de diagramas de secuencia
</commit_message>
<xml_diff>
--- a/Planeacion actividades.xlsx
+++ b/Planeacion actividades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrés\Universidad\SÉPTIMO SEMESTRE\FIS\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C7CA7-C6E9-46A0-BFAA-6665A445022C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89376C8B-40D8-4189-800B-594E1A5F9FE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{37E2385D-BCEF-49EC-9252-992955D84BB6}"/>
   </bookViews>
@@ -129,13 +129,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -145,6 +138,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFE3F39-B2D0-4C8D-A05F-5AE45C56E644}">
   <dimension ref="A2:N147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,31 +474,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <f>(SUM(E4:E7))</f>
         <v>10</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -508,95 +508,95 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="5">
+      <c r="B4" s="3"/>
+      <c r="C4" s="8">
         <v>43566</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="7">
         <v>43568</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4">
+      <c r="B5" s="5"/>
+      <c r="C5" s="7">
         <v>43569</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="7">
         <v>43572</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="4">
+      <c r="B6" s="3"/>
+      <c r="C6" s="7">
         <v>43573</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="7">
         <v>43573</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="4">
+      <c r="B7" s="5"/>
+      <c r="C7" s="7">
         <v>43574</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="8">
         <v>43575</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="3">
-        <f t="shared" ref="G8:G38" si="0">(SUM(E10:E13))</f>
+      <c r="G8" s="6">
+        <f t="shared" ref="G3:G38" si="0">(SUM(E10:E13))</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
@@ -607,194 +607,194 @@
         <v>7</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="5">
+      <c r="B10" s="3"/>
+      <c r="C10" s="8">
         <v>43576</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="7">
         <v>43577</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4">
+      <c r="B11" s="5"/>
+      <c r="C11" s="7">
         <v>43578</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="7">
         <v>43579</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="4">
+      <c r="B12" s="3"/>
+      <c r="C12" s="7">
         <v>43580</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="7">
         <v>43580</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="4">
+      <c r="B13" s="5"/>
+      <c r="C13" s="7">
         <v>43581</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="8">
         <v>43581</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="3"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="3" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="6">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="8">
+        <v>43582</v>
+      </c>
+      <c r="D16" s="7">
+        <v>43585</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="7">
+        <v>43586</v>
+      </c>
+      <c r="D17" s="7">
+        <v>43589</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="7">
+        <v>43590</v>
+      </c>
+      <c r="D18" s="7">
+        <v>43591</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="7">
+        <v>43592</v>
+      </c>
+      <c r="D19" s="8">
+        <v>43592</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5">
-        <v>43582</v>
-      </c>
-      <c r="D16" s="4">
-        <v>43585</v>
-      </c>
-      <c r="E16" s="1">
-        <v>4</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="4">
-        <v>43586</v>
-      </c>
-      <c r="D17" s="4">
-        <v>43592</v>
-      </c>
-      <c r="E17" s="1">
-        <v>7</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="4">
-        <v>43593</v>
-      </c>
-      <c r="D18" s="4">
-        <v>43593</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="4">
-        <v>43594</v>
-      </c>
-      <c r="D19" s="5">
-        <v>43594</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="3">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
@@ -805,95 +805,95 @@
         <v>7</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="3"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5">
-        <v>43565</v>
-      </c>
-      <c r="D22" s="4">
-        <v>43599</v>
+      <c r="B22" s="3"/>
+      <c r="C22" s="8">
+        <v>43563</v>
+      </c>
+      <c r="D22" s="7">
+        <v>43597</v>
       </c>
       <c r="E22" s="1">
         <v>5</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="4">
-        <v>43600</v>
-      </c>
-      <c r="D23" s="4">
-        <v>43604</v>
+      <c r="B23" s="5"/>
+      <c r="C23" s="7">
+        <v>43598</v>
+      </c>
+      <c r="D23" s="7">
+        <v>43602</v>
       </c>
       <c r="E23" s="1">
         <v>5</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="3"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="4">
-        <v>43605</v>
-      </c>
-      <c r="D24" s="4">
-        <v>43606</v>
+      <c r="B24" s="3"/>
+      <c r="C24" s="7">
+        <v>43603</v>
+      </c>
+      <c r="D24" s="7">
+        <v>43604</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="4">
-        <v>43607</v>
-      </c>
-      <c r="D25" s="5">
-        <v>43607</v>
+      <c r="B25" s="5"/>
+      <c r="C25" s="7">
+        <v>43605</v>
+      </c>
+      <c r="D25" s="8">
+        <v>43605</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="3"/>
+      <c r="G25" s="6"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
@@ -904,95 +904,95 @@
         <v>7</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="3"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="5">
-        <v>43608</v>
-      </c>
-      <c r="D28" s="4">
-        <v>43609</v>
+      <c r="B28" s="3"/>
+      <c r="C28" s="8">
+        <v>43606</v>
+      </c>
+      <c r="D28" s="7">
+        <v>43607</v>
       </c>
       <c r="E28" s="1">
         <v>2</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="4">
-        <v>43610</v>
-      </c>
-      <c r="D29" s="4">
-        <v>43611</v>
+      <c r="B29" s="5"/>
+      <c r="C29" s="7">
+        <v>43608</v>
+      </c>
+      <c r="D29" s="7">
+        <v>43609</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="4">
-        <v>43612</v>
-      </c>
-      <c r="D30" s="4">
-        <v>43612</v>
+      <c r="B30" s="3"/>
+      <c r="C30" s="7">
+        <v>43610</v>
+      </c>
+      <c r="D30" s="7">
+        <v>43610</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="4">
-        <v>43613</v>
-      </c>
-      <c r="D31" s="5">
-        <v>43613</v>
+      <c r="B31" s="5"/>
+      <c r="C31" s="7">
+        <v>43611</v>
+      </c>
+      <c r="D31" s="8">
+        <v>43611</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="3"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="3" t="s">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G32" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1003,95 +1003,95 @@
         <v>7</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="3"/>
+      <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="5">
-        <v>43614</v>
-      </c>
-      <c r="D34" s="4">
-        <v>43587</v>
+      <c r="B34" s="3"/>
+      <c r="C34" s="8">
+        <v>43612</v>
+      </c>
+      <c r="D34" s="7">
+        <v>43616</v>
       </c>
       <c r="E34" s="1">
         <v>5</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="3"/>
+      <c r="G34" s="6"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="4">
-        <v>43619</v>
-      </c>
-      <c r="D35" s="4">
-        <v>43623</v>
+      <c r="B35" s="5"/>
+      <c r="C35" s="7">
+        <v>43617</v>
+      </c>
+      <c r="D35" s="7">
+        <v>43621</v>
       </c>
       <c r="E35" s="1">
         <v>5</v>
       </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="3"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="4">
-        <v>43624</v>
-      </c>
-      <c r="D36" s="4">
-        <v>43625</v>
+      <c r="B36" s="3"/>
+      <c r="C36" s="7">
+        <v>43622</v>
+      </c>
+      <c r="D36" s="7">
+        <v>43623</v>
       </c>
       <c r="E36" s="1">
         <v>2</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="3"/>
+      <c r="G36" s="6"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="4">
-        <v>43626</v>
-      </c>
-      <c r="D37" s="5">
-        <v>43627</v>
+      <c r="B37" s="5"/>
+      <c r="C37" s="7">
+        <v>43624</v>
+      </c>
+      <c r="D37" s="8">
+        <v>43625</v>
       </c>
       <c r="E37" s="1">
         <v>2</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="3"/>
+      <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="3" t="s">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="3">
+      <c r="G38" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
       <c r="C39" s="1" t="s">
         <v>5</v>
       </c>
@@ -1104,15 +1104,15 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5">
-        <v>43628</v>
-      </c>
-      <c r="D40" s="4">
-        <v>43632</v>
+      <c r="B40" s="3"/>
+      <c r="C40" s="8">
+        <v>43626</v>
+      </c>
+      <c r="D40" s="7">
+        <v>43630</v>
       </c>
       <c r="E40" s="1">
         <v>5</v>
@@ -1120,15 +1120,15 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="4">
-        <v>43633</v>
-      </c>
-      <c r="D41" s="4">
-        <v>43637</v>
+      <c r="B41" s="5"/>
+      <c r="C41" s="7">
+        <v>43631</v>
+      </c>
+      <c r="D41" s="7">
+        <v>43635</v>
       </c>
       <c r="E41" s="1">
         <v>5</v>
@@ -1136,15 +1136,15 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="4">
-        <v>43638</v>
-      </c>
-      <c r="D42" s="4">
-        <v>43638</v>
+      <c r="B42" s="3"/>
+      <c r="C42" s="7">
+        <v>43636</v>
+      </c>
+      <c r="D42" s="7">
+        <v>43636</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -1152,15 +1152,15 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="4">
-        <v>43639</v>
-      </c>
-      <c r="D43" s="5">
-        <v>43639</v>
+      <c r="B43" s="5"/>
+      <c r="C43" s="7">
+        <v>43637</v>
+      </c>
+      <c r="D43" s="8">
+        <v>43637</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="G45">
         <f>SUM(G2:G44)</f>
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1799,10 +1799,23 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A9:B9"/>
@@ -1810,23 +1823,10 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrección del commit anterior
</commit_message>
<xml_diff>
--- a/Planeacion actividades.xlsx
+++ b/Planeacion actividades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andrés\Universidad\SÉPTIMO SEMESTRE\FIS\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89376C8B-40D8-4189-800B-594E1A5F9FE1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C7CA7-C6E9-46A0-BFAA-6665A445022C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{37E2385D-BCEF-49EC-9252-992955D84BB6}"/>
   </bookViews>
@@ -129,6 +129,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -138,13 +145,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BFE3F39-B2D0-4C8D-A05F-5AE45C56E644}">
   <dimension ref="A2:N147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,31 +474,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="3">
         <f>(SUM(E4:E7))</f>
         <v>10</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
@@ -508,95 +508,95 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="8">
+      <c r="B4" s="6"/>
+      <c r="C4" s="5">
         <v>43566</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="4">
         <v>43568</v>
       </c>
       <c r="E4" s="1">
         <v>3</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="7">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4">
         <v>43569</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <v>43572</v>
       </c>
       <c r="E5" s="1">
         <v>4</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="6"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="7">
+      <c r="B6" s="6"/>
+      <c r="C6" s="4">
         <v>43573</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <v>43573</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7">
+      <c r="B7" s="2"/>
+      <c r="C7" s="4">
         <v>43574</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <v>43575</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="6"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="6" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="6">
-        <f t="shared" ref="G3:G38" si="0">(SUM(E10:E13))</f>
+      <c r="G8" s="3">
+        <f t="shared" ref="G8:G38" si="0">(SUM(E10:E13))</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="1" t="s">
         <v>5</v>
       </c>
@@ -607,95 +607,95 @@
         <v>7</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="8">
+      <c r="B10" s="6"/>
+      <c r="C10" s="5">
         <v>43576</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>43577</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="7">
+      <c r="B11" s="2"/>
+      <c r="C11" s="4">
         <v>43578</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="4">
         <v>43579</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="6"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="7">
+      <c r="B12" s="6"/>
+      <c r="C12" s="4">
         <v>43580</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="4">
         <v>43580</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="7">
+      <c r="B13" s="2"/>
+      <c r="C13" s="4">
         <v>43581</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="5">
         <v>43581</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="6" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
@@ -706,95 +706,95 @@
         <v>7</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="8">
+      <c r="B16" s="6"/>
+      <c r="C16" s="5">
         <v>43582</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>43585</v>
       </c>
       <c r="E16" s="1">
         <v>4</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="7">
+      <c r="B17" s="2"/>
+      <c r="C17" s="4">
         <v>43586</v>
       </c>
-      <c r="D17" s="7">
-        <v>43589</v>
+      <c r="D17" s="4">
+        <v>43592</v>
       </c>
       <c r="E17" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="G17" s="6"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="7">
-        <v>43590</v>
-      </c>
-      <c r="D18" s="7">
-        <v>43591</v>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4">
+        <v>43593</v>
+      </c>
+      <c r="D18" s="4">
+        <v>43593</v>
       </c>
       <c r="E18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1"/>
-      <c r="G18" s="6"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="7">
-        <v>43592</v>
-      </c>
-      <c r="D19" s="8">
-        <v>43592</v>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4">
+        <v>43594</v>
+      </c>
+      <c r="D19" s="5">
+        <v>43594</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="6"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="6" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="1" t="s">
         <v>5</v>
       </c>
@@ -805,95 +805,95 @@
         <v>7</v>
       </c>
       <c r="F21" s="1"/>
-      <c r="G21" s="6"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="8">
-        <v>43563</v>
-      </c>
-      <c r="D22" s="7">
-        <v>43597</v>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5">
+        <v>43565</v>
+      </c>
+      <c r="D22" s="4">
+        <v>43599</v>
       </c>
       <c r="E22" s="1">
         <v>5</v>
       </c>
       <c r="F22" s="1"/>
-      <c r="G22" s="6"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="7">
-        <v>43598</v>
-      </c>
-      <c r="D23" s="7">
-        <v>43602</v>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4">
+        <v>43600</v>
+      </c>
+      <c r="D23" s="4">
+        <v>43604</v>
       </c>
       <c r="E23" s="1">
         <v>5</v>
       </c>
       <c r="F23" s="1"/>
-      <c r="G23" s="6"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="7">
-        <v>43603</v>
-      </c>
-      <c r="D24" s="7">
-        <v>43604</v>
+      <c r="B24" s="6"/>
+      <c r="C24" s="4">
+        <v>43605</v>
+      </c>
+      <c r="D24" s="4">
+        <v>43606</v>
       </c>
       <c r="E24" s="1">
         <v>2</v>
       </c>
       <c r="F24" s="1"/>
-      <c r="G24" s="6"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="7">
-        <v>43605</v>
-      </c>
-      <c r="D25" s="8">
-        <v>43605</v>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4">
+        <v>43607</v>
+      </c>
+      <c r="D25" s="5">
+        <v>43607</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25" s="1"/>
-      <c r="G25" s="6"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="6" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
@@ -904,95 +904,95 @@
         <v>7</v>
       </c>
       <c r="F27" s="1"/>
-      <c r="G27" s="6"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="8">
-        <v>43606</v>
-      </c>
-      <c r="D28" s="7">
-        <v>43607</v>
+      <c r="B28" s="6"/>
+      <c r="C28" s="5">
+        <v>43608</v>
+      </c>
+      <c r="D28" s="4">
+        <v>43609</v>
       </c>
       <c r="E28" s="1">
         <v>2</v>
       </c>
       <c r="F28" s="1"/>
-      <c r="G28" s="6"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="7">
-        <v>43608</v>
-      </c>
-      <c r="D29" s="7">
-        <v>43609</v>
+      <c r="B29" s="2"/>
+      <c r="C29" s="4">
+        <v>43610</v>
+      </c>
+      <c r="D29" s="4">
+        <v>43611</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
       </c>
       <c r="F29" s="1"/>
-      <c r="G29" s="6"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="7">
-        <v>43610</v>
-      </c>
-      <c r="D30" s="7">
-        <v>43610</v>
+      <c r="B30" s="6"/>
+      <c r="C30" s="4">
+        <v>43612</v>
+      </c>
+      <c r="D30" s="4">
+        <v>43612</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
       </c>
       <c r="F30" s="1"/>
-      <c r="G30" s="6"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="7">
-        <v>43611</v>
-      </c>
-      <c r="D31" s="8">
-        <v>43611</v>
+      <c r="B31" s="2"/>
+      <c r="C31" s="4">
+        <v>43613</v>
+      </c>
+      <c r="D31" s="5">
+        <v>43613</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="1"/>
-      <c r="G31" s="6"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="6" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="1" t="s">
         <v>5</v>
       </c>
@@ -1003,95 +1003,95 @@
         <v>7</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="6"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="8">
-        <v>43612</v>
-      </c>
-      <c r="D34" s="7">
-        <v>43616</v>
+      <c r="B34" s="6"/>
+      <c r="C34" s="5">
+        <v>43614</v>
+      </c>
+      <c r="D34" s="4">
+        <v>43587</v>
       </c>
       <c r="E34" s="1">
         <v>5</v>
       </c>
       <c r="F34" s="1"/>
-      <c r="G34" s="6"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="7">
-        <v>43617</v>
-      </c>
-      <c r="D35" s="7">
-        <v>43621</v>
+      <c r="B35" s="2"/>
+      <c r="C35" s="4">
+        <v>43619</v>
+      </c>
+      <c r="D35" s="4">
+        <v>43623</v>
       </c>
       <c r="E35" s="1">
         <v>5</v>
       </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="6"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="7">
-        <v>43622</v>
-      </c>
-      <c r="D36" s="7">
-        <v>43623</v>
+      <c r="B36" s="6"/>
+      <c r="C36" s="4">
+        <v>43624</v>
+      </c>
+      <c r="D36" s="4">
+        <v>43625</v>
       </c>
       <c r="E36" s="1">
         <v>2</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="6"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="7">
-        <v>43624</v>
-      </c>
-      <c r="D37" s="8">
-        <v>43625</v>
+      <c r="B37" s="2"/>
+      <c r="C37" s="4">
+        <v>43626</v>
+      </c>
+      <c r="D37" s="5">
+        <v>43627</v>
       </c>
       <c r="E37" s="1">
         <v>2</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="6"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="6" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="1" t="s">
         <v>5</v>
       </c>
@@ -1104,15 +1104,15 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="8">
-        <v>43626</v>
-      </c>
-      <c r="D40" s="7">
-        <v>43630</v>
+      <c r="B40" s="6"/>
+      <c r="C40" s="5">
+        <v>43628</v>
+      </c>
+      <c r="D40" s="4">
+        <v>43632</v>
       </c>
       <c r="E40" s="1">
         <v>5</v>
@@ -1120,15 +1120,15 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="7">
-        <v>43631</v>
-      </c>
-      <c r="D41" s="7">
-        <v>43635</v>
+      <c r="B41" s="2"/>
+      <c r="C41" s="4">
+        <v>43633</v>
+      </c>
+      <c r="D41" s="4">
+        <v>43637</v>
       </c>
       <c r="E41" s="1">
         <v>5</v>
@@ -1136,15 +1136,15 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="7">
-        <v>43636</v>
-      </c>
-      <c r="D42" s="7">
-        <v>43636</v>
+      <c r="B42" s="6"/>
+      <c r="C42" s="4">
+        <v>43638</v>
+      </c>
+      <c r="D42" s="4">
+        <v>43638</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
@@ -1152,15 +1152,15 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="7">
-        <v>43637</v>
-      </c>
-      <c r="D43" s="8">
-        <v>43637</v>
+      <c r="B43" s="2"/>
+      <c r="C43" s="4">
+        <v>43639</v>
+      </c>
+      <c r="D43" s="5">
+        <v>43639</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="G45">
         <f>SUM(G2:G44)</f>
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -1799,11 +1799,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A27:B27"/>
@@ -1811,22 +1822,11 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A39:B39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>